<commit_message>
updated gitignore and added sos
</commit_message>
<xml_diff>
--- a/Alumni_Fantasy_League.xlsx
+++ b/Alumni_Fantasy_League.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\PycharmProjects\Fantasy_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFD664A-A917-4F14-B5FC-DC7B7222D2A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64E86D7-5CEA-4EAF-A029-971CCCA1BFD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Points" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
   <si>
     <t>Week 1</t>
   </si>
@@ -154,6 +159,36 @@
   </si>
   <si>
     <t>Team Count</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
   </si>
 </sst>
 </file>
@@ -5685,7 +5720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P4" sqref="P4"/>
     </sheetView>
@@ -7271,10 +7306,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7443,11 +7478,880 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73">
+        <v>9</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="D79" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="14">
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A50:D50"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>